<commit_message>
Refactored code, properly handle formsubmission, currency validation, and alert on submission
</commit_message>
<xml_diff>
--- a/Website/public/RPA_CreatePurchaseRequestForm/PR_Form_Template.xlsx
+++ b/Website/public/RPA_CreatePurchaseRequestForm/PR_Form_Template.xlsx
@@ -5,10 +5,10 @@
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Abdul\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Abdul\Desktop\New folder (2)\RPA_CreatePurchaseRequestForm.1.0.23\content\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{08F234D5-A569-4DD2-B3B9-B9F3819913D8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01990280-4BDE-4D01-9CCF-EDEBB35E4200}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -329,13 +329,13 @@
     <t>OTHERS-Trading, PCB, Service, Office Use and etc</t>
   </si>
   <si>
-    <t xml:space="preserve">Doc No: </t>
-  </si>
-  <si>
     <t xml:space="preserve">Rev No: </t>
   </si>
   <si>
     <t>Signature</t>
+  </si>
+  <si>
+    <t>Doc No: QF-19</t>
   </si>
 </sst>
 </file>
@@ -345,10 +345,10 @@
   <numFmts count="6">
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="165" formatCode="[$-409]d\-mmm\-yy;@"/>
-    <numFmt numFmtId="166" formatCode="[$-409]d\-mmm\-yyyy;@"/>
-    <numFmt numFmtId="167" formatCode="&quot;RM&quot;#,##0.00"/>
-    <numFmt numFmtId="168" formatCode="[$MYR]\ #,##0.00;[$MYR]\ \-#,##0.00"/>
+    <numFmt numFmtId="164" formatCode="[$-409]d\-mmm\-yy;@"/>
+    <numFmt numFmtId="165" formatCode="[$-409]d\-mmm\-yyyy;@"/>
+    <numFmt numFmtId="166" formatCode="&quot;RM&quot;#,##0.00"/>
+    <numFmt numFmtId="167" formatCode="[$MYR]\ #,##0.00;[$MYR]\ \-#,##0.00"/>
   </numFmts>
   <fonts count="17">
     <font>
@@ -988,7 +988,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
@@ -1124,7 +1124,7 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="10" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="167" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1"/>
@@ -1183,13 +1183,13 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="168" fontId="6" fillId="0" borderId="5" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="6" fillId="0" borderId="5" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="168" fontId="7" fillId="0" borderId="5" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="7" fillId="0" borderId="5" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="9" fontId="6" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1211,13 +1211,22 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1228,152 +1237,24 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="6" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="6" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="6" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="6" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="166" fontId="6" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="6" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="21" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="22" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="4" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="6" fillId="4" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -1383,12 +1264,18 @@
     <xf numFmtId="0" fontId="6" fillId="4" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="4" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="4" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="4" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
@@ -1417,34 +1304,186 @@
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="21" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="22" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="6" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="6" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="6" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="6" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="6" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="6" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1454,45 +1493,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="7">
@@ -1814,8 +1814,8 @@
   </sheetPr>
   <dimension ref="A1:S70"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="B1" zoomScale="63" zoomScaleNormal="63" zoomScaleSheetLayoutView="115" workbookViewId="0">
-      <selection activeCell="S31" sqref="S31"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="63" zoomScaleNormal="63" zoomScaleSheetLayoutView="115" workbookViewId="0">
+      <selection activeCell="F7" sqref="F7:R7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>
@@ -1841,68 +1841,68 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:18" ht="18">
-      <c r="A1" s="103" t="s">
+      <c r="A1" s="142" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="104"/>
-      <c r="C1" s="104"/>
-      <c r="D1" s="104"/>
-      <c r="E1" s="104"/>
-      <c r="F1" s="104"/>
-      <c r="G1" s="104"/>
-      <c r="H1" s="104"/>
-      <c r="I1" s="104"/>
-      <c r="J1" s="104"/>
-      <c r="K1" s="104"/>
-      <c r="L1" s="104"/>
-      <c r="M1" s="104"/>
-      <c r="N1" s="104"/>
-      <c r="O1" s="104"/>
-      <c r="P1" s="104"/>
-      <c r="Q1" s="104"/>
-      <c r="R1" s="105"/>
+      <c r="B1" s="143"/>
+      <c r="C1" s="143"/>
+      <c r="D1" s="143"/>
+      <c r="E1" s="143"/>
+      <c r="F1" s="143"/>
+      <c r="G1" s="143"/>
+      <c r="H1" s="143"/>
+      <c r="I1" s="143"/>
+      <c r="J1" s="143"/>
+      <c r="K1" s="143"/>
+      <c r="L1" s="143"/>
+      <c r="M1" s="143"/>
+      <c r="N1" s="143"/>
+      <c r="O1" s="143"/>
+      <c r="P1" s="143"/>
+      <c r="Q1" s="143"/>
+      <c r="R1" s="144"/>
     </row>
     <row r="2" spans="1:18" ht="18">
-      <c r="A2" s="106" t="s">
+      <c r="A2" s="109" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="107"/>
-      <c r="C2" s="107"/>
-      <c r="D2" s="107"/>
-      <c r="E2" s="107"/>
-      <c r="F2" s="107"/>
-      <c r="G2" s="107"/>
-      <c r="H2" s="107"/>
-      <c r="I2" s="107"/>
-      <c r="J2" s="107"/>
-      <c r="K2" s="107"/>
-      <c r="L2" s="107"/>
-      <c r="M2" s="107"/>
-      <c r="N2" s="107"/>
-      <c r="O2" s="107"/>
-      <c r="P2" s="107"/>
-      <c r="Q2" s="107"/>
-      <c r="R2" s="108"/>
+      <c r="B2" s="110"/>
+      <c r="C2" s="110"/>
+      <c r="D2" s="110"/>
+      <c r="E2" s="110"/>
+      <c r="F2" s="110"/>
+      <c r="G2" s="110"/>
+      <c r="H2" s="110"/>
+      <c r="I2" s="110"/>
+      <c r="J2" s="110"/>
+      <c r="K2" s="110"/>
+      <c r="L2" s="110"/>
+      <c r="M2" s="110"/>
+      <c r="N2" s="110"/>
+      <c r="O2" s="110"/>
+      <c r="P2" s="110"/>
+      <c r="Q2" s="110"/>
+      <c r="R2" s="111"/>
     </row>
     <row r="3" spans="1:18" ht="18">
-      <c r="A3" s="109"/>
-      <c r="B3" s="110"/>
-      <c r="C3" s="110"/>
-      <c r="D3" s="110"/>
-      <c r="E3" s="110"/>
-      <c r="F3" s="110"/>
-      <c r="G3" s="110"/>
-      <c r="H3" s="110"/>
-      <c r="I3" s="110"/>
-      <c r="J3" s="110"/>
-      <c r="K3" s="110"/>
-      <c r="L3" s="110"/>
-      <c r="M3" s="110"/>
-      <c r="N3" s="110"/>
-      <c r="O3" s="110"/>
-      <c r="P3" s="110"/>
-      <c r="Q3" s="110"/>
-      <c r="R3" s="111"/>
+      <c r="A3" s="187"/>
+      <c r="B3" s="188"/>
+      <c r="C3" s="188"/>
+      <c r="D3" s="188"/>
+      <c r="E3" s="188"/>
+      <c r="F3" s="188"/>
+      <c r="G3" s="188"/>
+      <c r="H3" s="188"/>
+      <c r="I3" s="188"/>
+      <c r="J3" s="188"/>
+      <c r="K3" s="188"/>
+      <c r="L3" s="188"/>
+      <c r="M3" s="188"/>
+      <c r="N3" s="188"/>
+      <c r="O3" s="188"/>
+      <c r="P3" s="188"/>
+      <c r="Q3" s="188"/>
+      <c r="R3" s="189"/>
     </row>
     <row r="4" spans="1:18" ht="18">
       <c r="A4" s="28" t="s">
@@ -1929,7 +1929,7 @@
       <c r="P4" s="29"/>
       <c r="Q4" s="75"/>
       <c r="R4" s="87" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
     </row>
     <row r="5" spans="1:18" ht="18">
@@ -1951,14 +1951,14 @@
       <c r="P5" s="29"/>
       <c r="Q5" s="75"/>
       <c r="R5" s="87" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="6" spans="1:18" ht="18">
-      <c r="A6" s="112" t="s">
+      <c r="A6" s="190" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="113"/>
+      <c r="B6" s="191"/>
       <c r="C6" s="32" t="s">
         <v>6</v>
       </c>
@@ -1968,19 +1968,19 @@
       <c r="E6" s="31" t="s">
         <v>8</v>
       </c>
-      <c r="F6" s="114"/>
-      <c r="G6" s="115"/>
-      <c r="H6" s="115"/>
-      <c r="I6" s="115"/>
-      <c r="J6" s="115"/>
-      <c r="K6" s="115"/>
-      <c r="L6" s="115"/>
-      <c r="M6" s="115"/>
-      <c r="N6" s="115"/>
-      <c r="O6" s="115"/>
-      <c r="P6" s="115"/>
-      <c r="Q6" s="115"/>
-      <c r="R6" s="116"/>
+      <c r="F6" s="192"/>
+      <c r="G6" s="193"/>
+      <c r="H6" s="193"/>
+      <c r="I6" s="193"/>
+      <c r="J6" s="193"/>
+      <c r="K6" s="193"/>
+      <c r="L6" s="193"/>
+      <c r="M6" s="193"/>
+      <c r="N6" s="193"/>
+      <c r="O6" s="193"/>
+      <c r="P6" s="193"/>
+      <c r="Q6" s="193"/>
+      <c r="R6" s="194"/>
     </row>
     <row r="7" spans="1:18" ht="18">
       <c r="A7" s="34"/>
@@ -1990,106 +1990,106 @@
       <c r="E7" s="38" t="s">
         <v>10</v>
       </c>
-      <c r="F7" s="117"/>
-      <c r="G7" s="118"/>
-      <c r="H7" s="118"/>
-      <c r="I7" s="118"/>
-      <c r="J7" s="118"/>
-      <c r="K7" s="118"/>
-      <c r="L7" s="118"/>
-      <c r="M7" s="118"/>
-      <c r="N7" s="118"/>
-      <c r="O7" s="118"/>
-      <c r="P7" s="118"/>
-      <c r="Q7" s="118"/>
-      <c r="R7" s="119"/>
+      <c r="F7" s="179"/>
+      <c r="G7" s="180"/>
+      <c r="H7" s="180"/>
+      <c r="I7" s="180"/>
+      <c r="J7" s="180"/>
+      <c r="K7" s="180"/>
+      <c r="L7" s="180"/>
+      <c r="M7" s="180"/>
+      <c r="N7" s="180"/>
+      <c r="O7" s="180"/>
+      <c r="P7" s="180"/>
+      <c r="Q7" s="180"/>
+      <c r="R7" s="181"/>
     </row>
     <row r="8" spans="1:18" ht="18">
-      <c r="A8" s="120" t="s">
+      <c r="A8" s="182" t="s">
         <v>11</v>
       </c>
-      <c r="B8" s="121"/>
+      <c r="B8" s="183"/>
       <c r="C8" s="39"/>
       <c r="D8" s="40"/>
       <c r="E8" s="33" t="s">
         <v>12</v>
       </c>
-      <c r="F8" s="122"/>
-      <c r="G8" s="123"/>
-      <c r="H8" s="123"/>
-      <c r="I8" s="123"/>
-      <c r="J8" s="123"/>
-      <c r="K8" s="123"/>
-      <c r="L8" s="123"/>
-      <c r="M8" s="123"/>
-      <c r="N8" s="123"/>
-      <c r="O8" s="123"/>
-      <c r="P8" s="123"/>
-      <c r="Q8" s="123"/>
-      <c r="R8" s="124"/>
+      <c r="F8" s="184"/>
+      <c r="G8" s="185"/>
+      <c r="H8" s="185"/>
+      <c r="I8" s="185"/>
+      <c r="J8" s="185"/>
+      <c r="K8" s="185"/>
+      <c r="L8" s="185"/>
+      <c r="M8" s="185"/>
+      <c r="N8" s="185"/>
+      <c r="O8" s="185"/>
+      <c r="P8" s="185"/>
+      <c r="Q8" s="185"/>
+      <c r="R8" s="186"/>
     </row>
     <row r="9" spans="1:18" ht="18">
-      <c r="A9" s="125" t="s">
+      <c r="A9" s="166" t="s">
         <v>13</v>
       </c>
-      <c r="B9" s="126"/>
-      <c r="C9" s="127"/>
-      <c r="D9" s="128"/>
-      <c r="E9" s="128"/>
-      <c r="F9" s="128"/>
-      <c r="G9" s="128"/>
-      <c r="H9" s="128"/>
-      <c r="I9" s="128"/>
-      <c r="J9" s="128"/>
-      <c r="K9" s="128"/>
-      <c r="L9" s="128"/>
-      <c r="M9" s="128"/>
-      <c r="N9" s="128"/>
-      <c r="O9" s="128"/>
-      <c r="P9" s="128"/>
-      <c r="Q9" s="128"/>
-      <c r="R9" s="129"/>
+      <c r="B9" s="167"/>
+      <c r="C9" s="171"/>
+      <c r="D9" s="172"/>
+      <c r="E9" s="172"/>
+      <c r="F9" s="172"/>
+      <c r="G9" s="172"/>
+      <c r="H9" s="172"/>
+      <c r="I9" s="172"/>
+      <c r="J9" s="172"/>
+      <c r="K9" s="172"/>
+      <c r="L9" s="172"/>
+      <c r="M9" s="172"/>
+      <c r="N9" s="172"/>
+      <c r="O9" s="172"/>
+      <c r="P9" s="172"/>
+      <c r="Q9" s="172"/>
+      <c r="R9" s="178"/>
     </row>
     <row r="10" spans="1:18" ht="18">
-      <c r="A10" s="130" t="s">
+      <c r="A10" s="169" t="s">
         <v>15</v>
       </c>
-      <c r="B10" s="131"/>
-      <c r="C10" s="127"/>
-      <c r="D10" s="128"/>
-      <c r="E10" s="128"/>
-      <c r="F10" s="128"/>
-      <c r="G10" s="128"/>
-      <c r="H10" s="128"/>
-      <c r="I10" s="128"/>
-      <c r="J10" s="128"/>
-      <c r="K10" s="128"/>
-      <c r="L10" s="128"/>
-      <c r="M10" s="132"/>
-      <c r="N10" s="132"/>
-      <c r="O10" s="132"/>
-      <c r="P10" s="132"/>
-      <c r="Q10" s="132"/>
-      <c r="R10" s="133"/>
+      <c r="B10" s="170"/>
+      <c r="C10" s="171"/>
+      <c r="D10" s="172"/>
+      <c r="E10" s="172"/>
+      <c r="F10" s="172"/>
+      <c r="G10" s="172"/>
+      <c r="H10" s="172"/>
+      <c r="I10" s="172"/>
+      <c r="J10" s="172"/>
+      <c r="K10" s="172"/>
+      <c r="L10" s="172"/>
+      <c r="M10" s="173"/>
+      <c r="N10" s="173"/>
+      <c r="O10" s="173"/>
+      <c r="P10" s="173"/>
+      <c r="Q10" s="173"/>
+      <c r="R10" s="174"/>
     </row>
     <row r="11" spans="1:18" ht="37.950000000000003" customHeight="1">
-      <c r="A11" s="130" t="s">
+      <c r="A11" s="169" t="s">
         <v>16</v>
       </c>
-      <c r="B11" s="131"/>
-      <c r="C11" s="134" t="s">
+      <c r="B11" s="170"/>
+      <c r="C11" s="175" t="s">
         <v>17</v>
       </c>
-      <c r="D11" s="135"/>
+      <c r="D11" s="176"/>
       <c r="E11" s="42" t="s">
         <v>18</v>
       </c>
-      <c r="F11" s="136"/>
-      <c r="G11" s="128"/>
-      <c r="H11" s="128"/>
-      <c r="I11" s="128"/>
-      <c r="J11" s="128"/>
-      <c r="K11" s="129"/>
+      <c r="F11" s="177"/>
+      <c r="G11" s="172"/>
+      <c r="H11" s="172"/>
+      <c r="I11" s="172"/>
+      <c r="J11" s="172"/>
+      <c r="K11" s="178"/>
       <c r="L11" s="76" t="s">
         <v>19</v>
       </c>
@@ -2107,36 +2107,36 @@
       <c r="R11" s="77"/>
     </row>
     <row r="12" spans="1:18" ht="18">
-      <c r="A12" s="137" t="s">
+      <c r="A12" s="158" t="s">
         <v>23</v>
       </c>
-      <c r="B12" s="138"/>
-      <c r="C12" s="139" t="s">
+      <c r="B12" s="159"/>
+      <c r="C12" s="160" t="s">
         <v>17</v>
       </c>
-      <c r="D12" s="140"/>
+      <c r="D12" s="161"/>
       <c r="E12" s="38" t="s">
         <v>24</v>
       </c>
-      <c r="F12" s="141"/>
-      <c r="G12" s="142"/>
-      <c r="H12" s="142"/>
-      <c r="I12" s="142"/>
-      <c r="J12" s="142"/>
-      <c r="K12" s="142"/>
-      <c r="L12" s="142"/>
-      <c r="M12" s="143"/>
-      <c r="N12" s="143"/>
-      <c r="O12" s="143"/>
-      <c r="P12" s="143"/>
-      <c r="Q12" s="143"/>
-      <c r="R12" s="144"/>
+      <c r="F12" s="162"/>
+      <c r="G12" s="163"/>
+      <c r="H12" s="163"/>
+      <c r="I12" s="163"/>
+      <c r="J12" s="163"/>
+      <c r="K12" s="163"/>
+      <c r="L12" s="163"/>
+      <c r="M12" s="164"/>
+      <c r="N12" s="164"/>
+      <c r="O12" s="164"/>
+      <c r="P12" s="164"/>
+      <c r="Q12" s="164"/>
+      <c r="R12" s="165"/>
     </row>
     <row r="13" spans="1:18" ht="18">
-      <c r="A13" s="125" t="s">
+      <c r="A13" s="166" t="s">
         <v>25</v>
       </c>
-      <c r="B13" s="126"/>
+      <c r="B13" s="167"/>
       <c r="C13" s="44"/>
       <c r="D13" s="45"/>
       <c r="E13" s="45"/>
@@ -2164,10 +2164,10 @@
       <c r="C14" s="47" t="s">
         <v>28</v>
       </c>
-      <c r="D14" s="145" t="s">
+      <c r="D14" s="168" t="s">
         <v>29</v>
       </c>
-      <c r="E14" s="145"/>
+      <c r="E14" s="168"/>
       <c r="F14" s="48" t="s">
         <v>30</v>
       </c>
@@ -2214,8 +2214,8 @@
       </c>
       <c r="B15" s="50"/>
       <c r="C15" s="43"/>
-      <c r="D15" s="146"/>
-      <c r="E15" s="147"/>
+      <c r="D15" s="152"/>
+      <c r="E15" s="153"/>
       <c r="F15" s="52"/>
       <c r="G15" s="53"/>
       <c r="H15" s="53"/>
@@ -2236,8 +2236,8 @@
       </c>
       <c r="B16" s="51"/>
       <c r="C16" s="54"/>
-      <c r="D16" s="146"/>
-      <c r="E16" s="147"/>
+      <c r="D16" s="152"/>
+      <c r="E16" s="153"/>
       <c r="F16" s="52"/>
       <c r="G16" s="53"/>
       <c r="H16" s="53"/>
@@ -2258,8 +2258,8 @@
       </c>
       <c r="B17" s="51"/>
       <c r="C17" s="54"/>
-      <c r="D17" s="146"/>
-      <c r="E17" s="147"/>
+      <c r="D17" s="152"/>
+      <c r="E17" s="153"/>
       <c r="F17" s="52"/>
       <c r="G17" s="53"/>
       <c r="H17" s="53"/>
@@ -2280,8 +2280,8 @@
       </c>
       <c r="B18" s="51"/>
       <c r="C18" s="54"/>
-      <c r="D18" s="146"/>
-      <c r="E18" s="147"/>
+      <c r="D18" s="152"/>
+      <c r="E18" s="153"/>
       <c r="F18" s="52"/>
       <c r="G18" s="53"/>
       <c r="H18" s="53"/>
@@ -2302,8 +2302,8 @@
       </c>
       <c r="B19" s="51"/>
       <c r="C19" s="55"/>
-      <c r="D19" s="146"/>
-      <c r="E19" s="147"/>
+      <c r="D19" s="152"/>
+      <c r="E19" s="153"/>
       <c r="F19" s="52"/>
       <c r="G19" s="53"/>
       <c r="H19" s="53"/>
@@ -2324,8 +2324,8 @@
       </c>
       <c r="B20" s="51"/>
       <c r="C20" s="56"/>
-      <c r="D20" s="146"/>
-      <c r="E20" s="147"/>
+      <c r="D20" s="152"/>
+      <c r="E20" s="153"/>
       <c r="F20" s="52"/>
       <c r="G20" s="53"/>
       <c r="H20" s="53"/>
@@ -2346,8 +2346,8 @@
       </c>
       <c r="B21" s="43"/>
       <c r="C21" s="41"/>
-      <c r="D21" s="148"/>
-      <c r="E21" s="149"/>
+      <c r="D21" s="154"/>
+      <c r="E21" s="155"/>
       <c r="F21" s="52"/>
       <c r="G21" s="53"/>
       <c r="H21" s="57"/>
@@ -2368,8 +2368,8 @@
       </c>
       <c r="B22" s="43"/>
       <c r="C22" s="41"/>
-      <c r="D22" s="148"/>
-      <c r="E22" s="149"/>
+      <c r="D22" s="154"/>
+      <c r="E22" s="155"/>
       <c r="F22" s="52"/>
       <c r="G22" s="58"/>
       <c r="H22" s="53"/>
@@ -2390,8 +2390,8 @@
       </c>
       <c r="B23" s="43"/>
       <c r="C23" s="41"/>
-      <c r="D23" s="148"/>
-      <c r="E23" s="149"/>
+      <c r="D23" s="154"/>
+      <c r="E23" s="155"/>
       <c r="F23" s="52"/>
       <c r="G23" s="58"/>
       <c r="H23" s="53"/>
@@ -2412,8 +2412,8 @@
       </c>
       <c r="B24" s="41"/>
       <c r="C24" s="41"/>
-      <c r="D24" s="150"/>
-      <c r="E24" s="151"/>
+      <c r="D24" s="156"/>
+      <c r="E24" s="157"/>
       <c r="F24" s="59"/>
       <c r="G24" s="60"/>
       <c r="H24" s="61"/>
@@ -2434,10 +2434,10 @@
       </c>
       <c r="B25" s="49"/>
       <c r="C25" s="49"/>
-      <c r="D25" s="152" t="s">
+      <c r="D25" s="151" t="s">
         <v>40</v>
       </c>
-      <c r="E25" s="152"/>
+      <c r="E25" s="151"/>
       <c r="F25" s="62"/>
       <c r="G25" s="62"/>
       <c r="H25" s="62"/>
@@ -2475,21 +2475,21 @@
     <row r="27" spans="1:19" ht="18">
       <c r="A27" s="63"/>
       <c r="B27" s="29"/>
-      <c r="C27" s="189" t="s">
-        <v>94</v>
-      </c>
-      <c r="D27" s="190"/>
-      <c r="E27" s="185"/>
-      <c r="F27" s="187"/>
-      <c r="G27" s="185"/>
-      <c r="H27" s="186"/>
-      <c r="I27" s="187"/>
-      <c r="J27" s="185"/>
-      <c r="K27" s="186"/>
-      <c r="L27" s="187"/>
-      <c r="M27" s="185"/>
-      <c r="N27" s="186"/>
-      <c r="O27" s="187"/>
+      <c r="C27" s="112" t="s">
+        <v>93</v>
+      </c>
+      <c r="D27" s="113"/>
+      <c r="E27" s="103"/>
+      <c r="F27" s="105"/>
+      <c r="G27" s="103"/>
+      <c r="H27" s="104"/>
+      <c r="I27" s="105"/>
+      <c r="J27" s="103"/>
+      <c r="K27" s="104"/>
+      <c r="L27" s="105"/>
+      <c r="M27" s="103"/>
+      <c r="N27" s="104"/>
+      <c r="O27" s="105"/>
       <c r="P27" s="29"/>
       <c r="Q27" s="29"/>
       <c r="R27" s="29"/>
@@ -2497,19 +2497,19 @@
     <row r="28" spans="1:19" ht="18">
       <c r="A28" s="63"/>
       <c r="B28" s="29"/>
-      <c r="C28" s="191"/>
-      <c r="D28" s="192"/>
-      <c r="E28" s="188"/>
-      <c r="F28" s="175"/>
-      <c r="G28" s="188"/>
-      <c r="H28" s="174"/>
-      <c r="I28" s="175"/>
-      <c r="J28" s="188"/>
-      <c r="K28" s="174"/>
-      <c r="L28" s="175"/>
-      <c r="M28" s="188"/>
-      <c r="N28" s="174"/>
-      <c r="O28" s="175"/>
+      <c r="C28" s="114"/>
+      <c r="D28" s="115"/>
+      <c r="E28" s="106"/>
+      <c r="F28" s="108"/>
+      <c r="G28" s="106"/>
+      <c r="H28" s="107"/>
+      <c r="I28" s="108"/>
+      <c r="J28" s="106"/>
+      <c r="K28" s="107"/>
+      <c r="L28" s="108"/>
+      <c r="M28" s="106"/>
+      <c r="N28" s="107"/>
+      <c r="O28" s="108"/>
       <c r="P28" s="29"/>
       <c r="Q28" s="29" t="s">
         <v>41</v>
@@ -2519,19 +2519,19 @@
     <row r="29" spans="1:19" ht="18">
       <c r="A29" s="63"/>
       <c r="B29" s="29"/>
-      <c r="C29" s="193"/>
-      <c r="D29" s="194"/>
-      <c r="E29" s="106"/>
-      <c r="F29" s="108"/>
-      <c r="G29" s="106"/>
-      <c r="H29" s="107"/>
-      <c r="I29" s="108"/>
-      <c r="J29" s="106"/>
-      <c r="K29" s="107"/>
-      <c r="L29" s="108"/>
-      <c r="M29" s="106"/>
-      <c r="N29" s="107"/>
-      <c r="O29" s="108"/>
+      <c r="C29" s="116"/>
+      <c r="D29" s="117"/>
+      <c r="E29" s="109"/>
+      <c r="F29" s="111"/>
+      <c r="G29" s="109"/>
+      <c r="H29" s="110"/>
+      <c r="I29" s="111"/>
+      <c r="J29" s="109"/>
+      <c r="K29" s="110"/>
+      <c r="L29" s="111"/>
+      <c r="M29" s="109"/>
+      <c r="N29" s="110"/>
+      <c r="O29" s="111"/>
       <c r="P29" s="29"/>
       <c r="Q29" s="94" t="s">
         <v>42</v>
@@ -2542,29 +2542,29 @@
     <row r="30" spans="1:19" ht="18">
       <c r="A30" s="63"/>
       <c r="B30" s="29"/>
-      <c r="C30" s="103" t="s">
+      <c r="C30" s="142" t="s">
         <v>43</v>
       </c>
-      <c r="D30" s="105"/>
-      <c r="E30" s="103" t="s">
+      <c r="D30" s="144"/>
+      <c r="E30" s="142" t="s">
         <v>44</v>
       </c>
-      <c r="F30" s="105"/>
-      <c r="G30" s="103" t="s">
+      <c r="F30" s="144"/>
+      <c r="G30" s="142" t="s">
         <v>45</v>
       </c>
-      <c r="H30" s="104"/>
-      <c r="I30" s="105"/>
-      <c r="J30" s="103" t="s">
+      <c r="H30" s="143"/>
+      <c r="I30" s="144"/>
+      <c r="J30" s="142" t="s">
         <v>46</v>
       </c>
-      <c r="K30" s="104"/>
-      <c r="L30" s="105"/>
-      <c r="M30" s="103" t="s">
+      <c r="K30" s="143"/>
+      <c r="L30" s="144"/>
+      <c r="M30" s="142" t="s">
         <v>47</v>
       </c>
-      <c r="N30" s="104"/>
-      <c r="O30" s="105"/>
+      <c r="N30" s="143"/>
+      <c r="O30" s="144"/>
       <c r="P30" s="29"/>
       <c r="Q30" s="97" t="s">
         <v>48</v>
@@ -2585,11 +2585,11 @@
         <v>50</v>
       </c>
       <c r="F31" s="66"/>
-      <c r="G31" s="153" t="s">
+      <c r="G31" s="145" t="s">
         <v>51</v>
       </c>
-      <c r="H31" s="154"/>
-      <c r="I31" s="155"/>
+      <c r="H31" s="146"/>
+      <c r="I31" s="147"/>
       <c r="J31" s="28" t="s">
         <v>50</v>
       </c>
@@ -2620,11 +2620,11 @@
         <v>54</v>
       </c>
       <c r="F32" s="69"/>
-      <c r="G32" s="156" t="s">
+      <c r="G32" s="148" t="s">
         <v>54</v>
       </c>
-      <c r="H32" s="157"/>
-      <c r="I32" s="158"/>
+      <c r="H32" s="149"/>
+      <c r="I32" s="150"/>
       <c r="J32" s="67" t="s">
         <v>55</v>
       </c>
@@ -2642,30 +2642,30 @@
     </row>
     <row r="33" spans="1:19" ht="18">
       <c r="A33" s="63"/>
-      <c r="B33" s="174" t="s">
+      <c r="B33" s="107" t="s">
         <v>56</v>
       </c>
-      <c r="C33" s="174"/>
-      <c r="D33" s="175"/>
-      <c r="E33" s="159" t="s">
+      <c r="C33" s="107"/>
+      <c r="D33" s="108"/>
+      <c r="E33" s="127" t="s">
         <v>57</v>
       </c>
-      <c r="F33" s="160"/>
-      <c r="G33" s="159" t="s">
+      <c r="F33" s="128"/>
+      <c r="G33" s="127" t="s">
         <v>58</v>
       </c>
-      <c r="H33" s="161"/>
-      <c r="I33" s="160"/>
-      <c r="J33" s="159" t="s">
+      <c r="H33" s="129"/>
+      <c r="I33" s="128"/>
+      <c r="J33" s="127" t="s">
         <v>58</v>
       </c>
-      <c r="K33" s="161"/>
-      <c r="L33" s="160"/>
-      <c r="M33" s="159" t="s">
+      <c r="K33" s="129"/>
+      <c r="L33" s="128"/>
+      <c r="M33" s="127" t="s">
         <v>58</v>
       </c>
-      <c r="N33" s="161"/>
-      <c r="O33" s="160"/>
+      <c r="N33" s="129"/>
+      <c r="O33" s="128"/>
       <c r="P33" s="29"/>
       <c r="Q33" s="97" t="s">
         <v>59</v>
@@ -2677,28 +2677,28 @@
     </row>
     <row r="34" spans="1:19" ht="18">
       <c r="A34" s="63"/>
-      <c r="B34" s="174"/>
-      <c r="C34" s="174"/>
-      <c r="D34" s="175"/>
-      <c r="E34" s="159" t="s">
+      <c r="B34" s="107"/>
+      <c r="C34" s="107"/>
+      <c r="D34" s="108"/>
+      <c r="E34" s="127" t="s">
         <v>60</v>
       </c>
-      <c r="F34" s="160"/>
-      <c r="G34" s="159" t="s">
+      <c r="F34" s="128"/>
+      <c r="G34" s="127" t="s">
         <v>61</v>
       </c>
-      <c r="H34" s="161"/>
-      <c r="I34" s="160"/>
-      <c r="J34" s="159" t="s">
+      <c r="H34" s="129"/>
+      <c r="I34" s="128"/>
+      <c r="J34" s="127" t="s">
         <v>61</v>
       </c>
-      <c r="K34" s="161"/>
-      <c r="L34" s="160"/>
-      <c r="M34" s="159" t="s">
+      <c r="K34" s="129"/>
+      <c r="L34" s="128"/>
+      <c r="M34" s="127" t="s">
         <v>61</v>
       </c>
-      <c r="N34" s="161"/>
-      <c r="O34" s="160"/>
+      <c r="N34" s="129"/>
+      <c r="O34" s="128"/>
       <c r="P34" s="29"/>
       <c r="Q34" s="94"/>
       <c r="R34" s="100" t="s">
@@ -2731,21 +2731,21 @@
     <row r="36" spans="1:19" ht="18">
       <c r="A36" s="63"/>
       <c r="B36" s="63"/>
-      <c r="C36" s="176" t="s">
+      <c r="C36" s="133" t="s">
         <v>62</v>
       </c>
-      <c r="D36" s="177"/>
-      <c r="E36" s="177"/>
-      <c r="F36" s="177"/>
-      <c r="G36" s="177"/>
-      <c r="H36" s="177"/>
-      <c r="I36" s="177"/>
-      <c r="J36" s="177"/>
-      <c r="K36" s="177"/>
-      <c r="L36" s="177"/>
-      <c r="M36" s="177"/>
-      <c r="N36" s="177"/>
-      <c r="O36" s="178"/>
+      <c r="D36" s="134"/>
+      <c r="E36" s="134"/>
+      <c r="F36" s="134"/>
+      <c r="G36" s="134"/>
+      <c r="H36" s="134"/>
+      <c r="I36" s="134"/>
+      <c r="J36" s="134"/>
+      <c r="K36" s="134"/>
+      <c r="L36" s="134"/>
+      <c r="M36" s="134"/>
+      <c r="N36" s="134"/>
+      <c r="O36" s="135"/>
       <c r="P36" s="29"/>
       <c r="Q36" s="29"/>
       <c r="R36" s="29"/>
@@ -2753,19 +2753,19 @@
     <row r="37" spans="1:19" ht="18">
       <c r="A37" s="63"/>
       <c r="B37" s="63"/>
-      <c r="C37" s="179"/>
-      <c r="D37" s="180"/>
-      <c r="E37" s="180"/>
-      <c r="F37" s="180"/>
-      <c r="G37" s="180"/>
-      <c r="H37" s="180"/>
-      <c r="I37" s="180"/>
-      <c r="J37" s="180"/>
-      <c r="K37" s="180"/>
-      <c r="L37" s="180"/>
-      <c r="M37" s="180"/>
-      <c r="N37" s="180"/>
-      <c r="O37" s="181"/>
+      <c r="C37" s="136"/>
+      <c r="D37" s="137"/>
+      <c r="E37" s="137"/>
+      <c r="F37" s="137"/>
+      <c r="G37" s="137"/>
+      <c r="H37" s="137"/>
+      <c r="I37" s="137"/>
+      <c r="J37" s="137"/>
+      <c r="K37" s="137"/>
+      <c r="L37" s="137"/>
+      <c r="M37" s="137"/>
+      <c r="N37" s="137"/>
+      <c r="O37" s="138"/>
       <c r="P37" s="29"/>
       <c r="Q37" s="29"/>
       <c r="R37" s="29"/>
@@ -2773,19 +2773,19 @@
     <row r="38" spans="1:19" ht="18">
       <c r="A38" s="29"/>
       <c r="B38" s="29"/>
-      <c r="C38" s="179"/>
-      <c r="D38" s="180"/>
-      <c r="E38" s="180"/>
-      <c r="F38" s="180"/>
-      <c r="G38" s="180"/>
-      <c r="H38" s="180"/>
-      <c r="I38" s="180"/>
-      <c r="J38" s="180"/>
-      <c r="K38" s="180"/>
-      <c r="L38" s="180"/>
-      <c r="M38" s="180"/>
-      <c r="N38" s="180"/>
-      <c r="O38" s="181"/>
+      <c r="C38" s="136"/>
+      <c r="D38" s="137"/>
+      <c r="E38" s="137"/>
+      <c r="F38" s="137"/>
+      <c r="G38" s="137"/>
+      <c r="H38" s="137"/>
+      <c r="I38" s="137"/>
+      <c r="J38" s="137"/>
+      <c r="K38" s="137"/>
+      <c r="L38" s="137"/>
+      <c r="M38" s="137"/>
+      <c r="N38" s="137"/>
+      <c r="O38" s="138"/>
       <c r="P38" s="29"/>
       <c r="Q38" s="29"/>
       <c r="R38" s="29"/>
@@ -2793,19 +2793,19 @@
     <row r="39" spans="1:19" ht="20.399999999999999">
       <c r="A39" s="70"/>
       <c r="B39" s="29"/>
-      <c r="C39" s="182"/>
-      <c r="D39" s="183"/>
-      <c r="E39" s="183"/>
-      <c r="F39" s="183"/>
-      <c r="G39" s="183"/>
-      <c r="H39" s="183"/>
-      <c r="I39" s="183"/>
-      <c r="J39" s="183"/>
-      <c r="K39" s="183"/>
-      <c r="L39" s="183"/>
-      <c r="M39" s="183"/>
-      <c r="N39" s="183"/>
-      <c r="O39" s="184"/>
+      <c r="C39" s="139"/>
+      <c r="D39" s="140"/>
+      <c r="E39" s="140"/>
+      <c r="F39" s="140"/>
+      <c r="G39" s="140"/>
+      <c r="H39" s="140"/>
+      <c r="I39" s="140"/>
+      <c r="J39" s="140"/>
+      <c r="K39" s="140"/>
+      <c r="L39" s="140"/>
+      <c r="M39" s="140"/>
+      <c r="N39" s="140"/>
+      <c r="O39" s="141"/>
       <c r="P39" s="29"/>
       <c r="Q39" s="29"/>
       <c r="R39" s="29"/>
@@ -2831,13 +2831,13 @@
     </row>
     <row r="41" spans="1:19" ht="18">
       <c r="A41" s="71"/>
-      <c r="B41" s="162" t="s">
+      <c r="B41" s="130" t="s">
         <v>63</v>
       </c>
-      <c r="C41" s="163"/>
-      <c r="D41" s="163"/>
-      <c r="E41" s="163"/>
-      <c r="F41" s="164"/>
+      <c r="C41" s="131"/>
+      <c r="D41" s="131"/>
+      <c r="E41" s="131"/>
+      <c r="F41" s="132"/>
       <c r="G41" s="71"/>
       <c r="H41" s="29"/>
       <c r="I41" s="29"/>
@@ -2853,13 +2853,13 @@
     </row>
     <row r="42" spans="1:19" ht="18">
       <c r="A42" s="71"/>
-      <c r="B42" s="165" t="s">
+      <c r="B42" s="118" t="s">
         <v>64</v>
       </c>
-      <c r="C42" s="166"/>
-      <c r="D42" s="166"/>
-      <c r="E42" s="166"/>
-      <c r="F42" s="167"/>
+      <c r="C42" s="119"/>
+      <c r="D42" s="119"/>
+      <c r="E42" s="119"/>
+      <c r="F42" s="120"/>
       <c r="G42" s="71"/>
       <c r="H42" s="29"/>
       <c r="I42" s="29"/>
@@ -2875,13 +2875,13 @@
     </row>
     <row r="43" spans="1:19" ht="18">
       <c r="A43" s="73"/>
-      <c r="B43" s="168" t="s">
+      <c r="B43" s="121" t="s">
         <v>65</v>
       </c>
-      <c r="C43" s="169"/>
-      <c r="D43" s="169"/>
-      <c r="E43" s="169"/>
-      <c r="F43" s="170"/>
+      <c r="C43" s="122"/>
+      <c r="D43" s="122"/>
+      <c r="E43" s="122"/>
+      <c r="F43" s="123"/>
       <c r="G43" s="73"/>
       <c r="H43" s="29"/>
       <c r="I43" s="29"/>
@@ -2897,13 +2897,13 @@
     </row>
     <row r="44" spans="1:19" ht="18">
       <c r="A44" s="29"/>
-      <c r="B44" s="165" t="s">
+      <c r="B44" s="118" t="s">
         <v>66</v>
       </c>
-      <c r="C44" s="166"/>
-      <c r="D44" s="166"/>
-      <c r="E44" s="166"/>
-      <c r="F44" s="167"/>
+      <c r="C44" s="119"/>
+      <c r="D44" s="119"/>
+      <c r="E44" s="119"/>
+      <c r="F44" s="120"/>
       <c r="G44" s="29"/>
       <c r="H44" s="29"/>
       <c r="I44" s="29"/>
@@ -2919,13 +2919,13 @@
     </row>
     <row r="45" spans="1:19" ht="18">
       <c r="A45" s="29"/>
-      <c r="B45" s="165" t="s">
+      <c r="B45" s="118" t="s">
         <v>67</v>
       </c>
-      <c r="C45" s="166"/>
-      <c r="D45" s="166"/>
-      <c r="E45" s="166"/>
-      <c r="F45" s="167"/>
+      <c r="C45" s="119"/>
+      <c r="D45" s="119"/>
+      <c r="E45" s="119"/>
+      <c r="F45" s="120"/>
       <c r="G45" s="29"/>
       <c r="H45" s="29"/>
       <c r="I45" s="29"/>
@@ -2940,13 +2940,13 @@
       <c r="R45" s="29"/>
     </row>
     <row r="46" spans="1:19" ht="18">
-      <c r="B46" s="171" t="s">
+      <c r="B46" s="124" t="s">
         <v>68</v>
       </c>
-      <c r="C46" s="172"/>
-      <c r="D46" s="172"/>
-      <c r="E46" s="172"/>
-      <c r="F46" s="173"/>
+      <c r="C46" s="125"/>
+      <c r="D46" s="125"/>
+      <c r="E46" s="125"/>
+      <c r="F46" s="126"/>
     </row>
     <row r="69" spans="5:9">
       <c r="E69" s="22"/>
@@ -2964,28 +2964,36 @@
     </row>
   </sheetData>
   <mergeCells count="59">
-    <mergeCell ref="M27:O29"/>
-    <mergeCell ref="C27:D29"/>
-    <mergeCell ref="E27:F29"/>
-    <mergeCell ref="B42:F42"/>
-    <mergeCell ref="B43:F43"/>
-    <mergeCell ref="B44:F44"/>
-    <mergeCell ref="B45:F45"/>
-    <mergeCell ref="B46:F46"/>
-    <mergeCell ref="E34:F34"/>
-    <mergeCell ref="G34:I34"/>
-    <mergeCell ref="J34:L34"/>
-    <mergeCell ref="M34:O34"/>
-    <mergeCell ref="B41:F41"/>
-    <mergeCell ref="B33:D34"/>
-    <mergeCell ref="C36:O39"/>
-    <mergeCell ref="M30:O30"/>
-    <mergeCell ref="G31:I31"/>
-    <mergeCell ref="G32:I32"/>
-    <mergeCell ref="E33:F33"/>
-    <mergeCell ref="G33:I33"/>
-    <mergeCell ref="J33:L33"/>
-    <mergeCell ref="M33:O33"/>
+    <mergeCell ref="A1:R1"/>
+    <mergeCell ref="A2:R2"/>
+    <mergeCell ref="A3:R3"/>
+    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="F6:R6"/>
+    <mergeCell ref="F7:R7"/>
+    <mergeCell ref="A8:B8"/>
+    <mergeCell ref="F8:R8"/>
+    <mergeCell ref="A9:B9"/>
+    <mergeCell ref="C9:R9"/>
+    <mergeCell ref="A10:B10"/>
+    <mergeCell ref="C10:R10"/>
+    <mergeCell ref="A11:B11"/>
+    <mergeCell ref="C11:D11"/>
+    <mergeCell ref="F11:K11"/>
+    <mergeCell ref="A12:B12"/>
+    <mergeCell ref="C12:D12"/>
+    <mergeCell ref="F12:R12"/>
+    <mergeCell ref="A13:B13"/>
+    <mergeCell ref="D14:E14"/>
+    <mergeCell ref="D15:E15"/>
+    <mergeCell ref="D16:E16"/>
+    <mergeCell ref="D17:E17"/>
+    <mergeCell ref="D18:E18"/>
+    <mergeCell ref="D19:E19"/>
+    <mergeCell ref="D20:E20"/>
+    <mergeCell ref="D21:E21"/>
+    <mergeCell ref="D22:E22"/>
+    <mergeCell ref="D23:E23"/>
+    <mergeCell ref="D24:E24"/>
     <mergeCell ref="D25:E25"/>
     <mergeCell ref="C30:D30"/>
     <mergeCell ref="E30:F30"/>
@@ -2993,36 +3001,28 @@
     <mergeCell ref="J30:L30"/>
     <mergeCell ref="G27:I29"/>
     <mergeCell ref="J27:L29"/>
-    <mergeCell ref="D20:E20"/>
-    <mergeCell ref="D21:E21"/>
-    <mergeCell ref="D22:E22"/>
-    <mergeCell ref="D23:E23"/>
-    <mergeCell ref="D24:E24"/>
-    <mergeCell ref="D15:E15"/>
-    <mergeCell ref="D16:E16"/>
-    <mergeCell ref="D17:E17"/>
-    <mergeCell ref="D18:E18"/>
-    <mergeCell ref="D19:E19"/>
-    <mergeCell ref="A12:B12"/>
-    <mergeCell ref="C12:D12"/>
-    <mergeCell ref="F12:R12"/>
-    <mergeCell ref="A13:B13"/>
-    <mergeCell ref="D14:E14"/>
-    <mergeCell ref="A10:B10"/>
-    <mergeCell ref="C10:R10"/>
-    <mergeCell ref="A11:B11"/>
-    <mergeCell ref="C11:D11"/>
-    <mergeCell ref="F11:K11"/>
-    <mergeCell ref="F7:R7"/>
-    <mergeCell ref="A8:B8"/>
-    <mergeCell ref="F8:R8"/>
-    <mergeCell ref="A9:B9"/>
-    <mergeCell ref="C9:R9"/>
-    <mergeCell ref="A1:R1"/>
-    <mergeCell ref="A2:R2"/>
-    <mergeCell ref="A3:R3"/>
-    <mergeCell ref="A6:B6"/>
-    <mergeCell ref="F6:R6"/>
+    <mergeCell ref="B44:F44"/>
+    <mergeCell ref="B45:F45"/>
+    <mergeCell ref="B46:F46"/>
+    <mergeCell ref="E34:F34"/>
+    <mergeCell ref="G34:I34"/>
+    <mergeCell ref="B41:F41"/>
+    <mergeCell ref="B33:D34"/>
+    <mergeCell ref="C36:O39"/>
+    <mergeCell ref="E33:F33"/>
+    <mergeCell ref="G33:I33"/>
+    <mergeCell ref="J33:L33"/>
+    <mergeCell ref="M33:O33"/>
+    <mergeCell ref="M27:O29"/>
+    <mergeCell ref="C27:D29"/>
+    <mergeCell ref="E27:F29"/>
+    <mergeCell ref="B42:F42"/>
+    <mergeCell ref="B43:F43"/>
+    <mergeCell ref="J34:L34"/>
+    <mergeCell ref="M34:O34"/>
+    <mergeCell ref="M30:O30"/>
+    <mergeCell ref="G31:I31"/>
+    <mergeCell ref="G32:I32"/>
   </mergeCells>
   <dataValidations count="3">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="K4 N4" xr:uid="{00000000-0002-0000-0000-000000000000}">
@@ -3060,83 +3060,83 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9">
-      <c r="A1" s="195" t="s">
+      <c r="A1" s="208" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="195"/>
-      <c r="C1" s="195"/>
-      <c r="D1" s="195"/>
-      <c r="E1" s="195"/>
-      <c r="F1" s="195"/>
-      <c r="G1" s="195"/>
-      <c r="H1" s="195"/>
-      <c r="I1" s="195"/>
+      <c r="B1" s="208"/>
+      <c r="C1" s="208"/>
+      <c r="D1" s="208"/>
+      <c r="E1" s="208"/>
+      <c r="F1" s="208"/>
+      <c r="G1" s="208"/>
+      <c r="H1" s="208"/>
+      <c r="I1" s="208"/>
     </row>
     <row r="2" spans="1:9" ht="46.5" customHeight="1">
-      <c r="A2" s="196" t="s">
+      <c r="A2" s="209" t="s">
         <v>69</v>
       </c>
-      <c r="B2" s="196"/>
-      <c r="C2" s="196"/>
-      <c r="D2" s="196"/>
-      <c r="E2" s="196"/>
-      <c r="F2" s="196"/>
-      <c r="G2" s="196"/>
-      <c r="H2" s="196"/>
-      <c r="I2" s="196"/>
+      <c r="B2" s="209"/>
+      <c r="C2" s="209"/>
+      <c r="D2" s="209"/>
+      <c r="E2" s="209"/>
+      <c r="F2" s="209"/>
+      <c r="G2" s="209"/>
+      <c r="H2" s="209"/>
+      <c r="I2" s="209"/>
     </row>
     <row r="3" spans="1:9">
-      <c r="A3" s="197"/>
-      <c r="B3" s="197"/>
-      <c r="C3" s="197"/>
-      <c r="D3" s="197"/>
-      <c r="E3" s="197"/>
-      <c r="F3" s="197"/>
-      <c r="G3" s="197"/>
-      <c r="H3" s="197"/>
-      <c r="I3" s="197"/>
+      <c r="A3" s="210"/>
+      <c r="B3" s="210"/>
+      <c r="C3" s="210"/>
+      <c r="D3" s="210"/>
+      <c r="E3" s="210"/>
+      <c r="F3" s="210"/>
+      <c r="G3" s="210"/>
+      <c r="H3" s="210"/>
+      <c r="I3" s="210"/>
     </row>
     <row r="4" spans="1:9">
-      <c r="A4" s="198"/>
-      <c r="B4" s="198"/>
-      <c r="C4" s="198"/>
-      <c r="D4" s="198"/>
-      <c r="E4" s="198"/>
-      <c r="F4" s="198"/>
-      <c r="G4" s="198"/>
-      <c r="H4" s="198"/>
-      <c r="I4" s="198"/>
+      <c r="A4" s="195"/>
+      <c r="B4" s="195"/>
+      <c r="C4" s="195"/>
+      <c r="D4" s="195"/>
+      <c r="E4" s="195"/>
+      <c r="F4" s="195"/>
+      <c r="G4" s="195"/>
+      <c r="H4" s="195"/>
+      <c r="I4" s="195"/>
     </row>
     <row r="5" spans="1:9">
-      <c r="A5" s="199" t="s">
+      <c r="A5" s="202" t="s">
         <v>18</v>
       </c>
-      <c r="B5" s="199"/>
-      <c r="C5" s="197"/>
-      <c r="D5" s="197"/>
-      <c r="E5" s="197"/>
-      <c r="F5" s="197"/>
-      <c r="G5" s="197"/>
-      <c r="H5" s="199"/>
-      <c r="I5" s="199"/>
+      <c r="B5" s="202"/>
+      <c r="C5" s="210"/>
+      <c r="D5" s="210"/>
+      <c r="E5" s="210"/>
+      <c r="F5" s="210"/>
+      <c r="G5" s="210"/>
+      <c r="H5" s="202"/>
+      <c r="I5" s="202"/>
     </row>
     <row r="6" spans="1:9">
-      <c r="A6" s="199"/>
-      <c r="B6" s="199"/>
-      <c r="C6" s="199"/>
-      <c r="D6" s="199"/>
-      <c r="E6" s="199"/>
-      <c r="F6" s="199"/>
-      <c r="G6" s="199"/>
-      <c r="H6" s="199"/>
-      <c r="I6" s="199"/>
+      <c r="A6" s="202"/>
+      <c r="B6" s="202"/>
+      <c r="C6" s="202"/>
+      <c r="D6" s="202"/>
+      <c r="E6" s="202"/>
+      <c r="F6" s="202"/>
+      <c r="G6" s="202"/>
+      <c r="H6" s="202"/>
+      <c r="I6" s="202"/>
     </row>
     <row r="7" spans="1:9">
-      <c r="A7" s="203" t="s">
+      <c r="A7" s="196" t="s">
         <v>70</v>
       </c>
-      <c r="B7" s="204"/>
-      <c r="C7" s="205"/>
+      <c r="B7" s="197"/>
+      <c r="C7" s="198"/>
       <c r="D7" s="3" t="s">
         <v>7</v>
       </c>
@@ -3152,9 +3152,9 @@
       </c>
     </row>
     <row r="8" spans="1:9">
-      <c r="A8" s="206"/>
-      <c r="B8" s="207"/>
-      <c r="C8" s="208"/>
+      <c r="A8" s="199"/>
+      <c r="B8" s="200"/>
+      <c r="C8" s="201"/>
       <c r="D8" s="5" t="s">
         <v>9</v>
       </c>
@@ -3164,27 +3164,27 @@
       <c r="H8" s="7"/>
     </row>
     <row r="9" spans="1:9" ht="51" customHeight="1">
-      <c r="A9" s="200" t="s">
+      <c r="A9" s="205" t="s">
         <v>73</v>
       </c>
-      <c r="B9" s="200"/>
-      <c r="C9" s="200"/>
-      <c r="D9" s="200"/>
-      <c r="E9" s="200"/>
-      <c r="F9" s="200"/>
-      <c r="G9" s="200"/>
-      <c r="H9" s="200"/>
-      <c r="I9" s="200"/>
+      <c r="B9" s="205"/>
+      <c r="C9" s="205"/>
+      <c r="D9" s="205"/>
+      <c r="E9" s="205"/>
+      <c r="F9" s="205"/>
+      <c r="G9" s="205"/>
+      <c r="H9" s="205"/>
+      <c r="I9" s="205"/>
     </row>
     <row r="10" spans="1:9">
       <c r="A10" s="8" t="s">
         <v>74</v>
       </c>
-      <c r="B10" s="201" t="s">
+      <c r="B10" s="206" t="s">
         <v>29</v>
       </c>
-      <c r="C10" s="201"/>
-      <c r="D10" s="201"/>
+      <c r="C10" s="206"/>
+      <c r="D10" s="206"/>
       <c r="E10" s="9" t="s">
         <v>31</v>
       </c>
@@ -3391,93 +3391,100 @@
       <c r="I26" s="26"/>
     </row>
     <row r="27" spans="1:9" ht="48" customHeight="1">
-      <c r="A27" s="202" t="s">
+      <c r="A27" s="207" t="s">
         <v>84</v>
       </c>
-      <c r="B27" s="202"/>
-      <c r="C27" s="202"/>
-      <c r="D27" s="202"/>
-      <c r="E27" s="202"/>
-      <c r="F27" s="202"/>
-      <c r="G27" s="202"/>
-      <c r="H27" s="202"/>
-      <c r="I27" s="202"/>
+      <c r="B27" s="207"/>
+      <c r="C27" s="207"/>
+      <c r="D27" s="207"/>
+      <c r="E27" s="207"/>
+      <c r="F27" s="207"/>
+      <c r="G27" s="207"/>
+      <c r="H27" s="207"/>
+      <c r="I27" s="207"/>
     </row>
     <row r="28" spans="1:9">
-      <c r="A28" s="199" t="s">
+      <c r="A28" s="202" t="s">
         <v>0</v>
       </c>
-      <c r="B28" s="199"/>
-      <c r="C28" s="199"/>
-      <c r="D28" s="199"/>
-      <c r="E28" s="199"/>
-      <c r="F28" s="199"/>
-      <c r="G28" s="199"/>
-      <c r="H28" s="199"/>
-      <c r="I28" s="199"/>
+      <c r="B28" s="202"/>
+      <c r="C28" s="202"/>
+      <c r="D28" s="202"/>
+      <c r="E28" s="202"/>
+      <c r="F28" s="202"/>
+      <c r="G28" s="202"/>
+      <c r="H28" s="202"/>
+      <c r="I28" s="202"/>
     </row>
     <row r="29" spans="1:9">
-      <c r="A29" s="209">
+      <c r="A29" s="203">
         <f>E8</f>
         <v>0</v>
       </c>
-      <c r="B29" s="209"/>
-      <c r="C29" s="209"/>
-      <c r="D29" s="199"/>
-      <c r="E29" s="199"/>
-      <c r="F29" s="199"/>
-      <c r="G29" s="199"/>
-      <c r="H29" s="199"/>
-      <c r="I29" s="199"/>
+      <c r="B29" s="203"/>
+      <c r="C29" s="203"/>
+      <c r="D29" s="202"/>
+      <c r="E29" s="202"/>
+      <c r="F29" s="202"/>
+      <c r="G29" s="202"/>
+      <c r="H29" s="202"/>
+      <c r="I29" s="202"/>
     </row>
     <row r="30" spans="1:9">
-      <c r="A30" s="209"/>
-      <c r="B30" s="209"/>
-      <c r="C30" s="209"/>
-      <c r="D30" s="199"/>
-      <c r="E30" s="199"/>
-      <c r="F30" s="199"/>
-      <c r="G30" s="199"/>
-      <c r="H30" s="199"/>
-      <c r="I30" s="199"/>
+      <c r="A30" s="203"/>
+      <c r="B30" s="203"/>
+      <c r="C30" s="203"/>
+      <c r="D30" s="202"/>
+      <c r="E30" s="202"/>
+      <c r="F30" s="202"/>
+      <c r="G30" s="202"/>
+      <c r="H30" s="202"/>
+      <c r="I30" s="202"/>
     </row>
     <row r="31" spans="1:9">
-      <c r="A31" s="209"/>
-      <c r="B31" s="209"/>
-      <c r="C31" s="209"/>
-      <c r="D31" s="199"/>
-      <c r="E31" s="199"/>
-      <c r="F31" s="199"/>
-      <c r="G31" s="199"/>
-      <c r="H31" s="199"/>
-      <c r="I31" s="199"/>
+      <c r="A31" s="203"/>
+      <c r="B31" s="203"/>
+      <c r="C31" s="203"/>
+      <c r="D31" s="202"/>
+      <c r="E31" s="202"/>
+      <c r="F31" s="202"/>
+      <c r="G31" s="202"/>
+      <c r="H31" s="202"/>
+      <c r="I31" s="202"/>
     </row>
     <row r="32" spans="1:9">
-      <c r="A32" s="210"/>
-      <c r="B32" s="210"/>
-      <c r="C32" s="210"/>
-      <c r="D32" s="199"/>
-      <c r="E32" s="199"/>
-      <c r="F32" s="199"/>
-      <c r="G32" s="199"/>
-      <c r="H32" s="199"/>
-      <c r="I32" s="199"/>
+      <c r="A32" s="204"/>
+      <c r="B32" s="204"/>
+      <c r="C32" s="204"/>
+      <c r="D32" s="202"/>
+      <c r="E32" s="202"/>
+      <c r="F32" s="202"/>
+      <c r="G32" s="202"/>
+      <c r="H32" s="202"/>
+      <c r="I32" s="202"/>
     </row>
     <row r="33" spans="1:9">
-      <c r="A33" s="198" t="s">
+      <c r="A33" s="195" t="s">
         <v>85</v>
       </c>
-      <c r="B33" s="198"/>
-      <c r="C33" s="198"/>
-      <c r="D33" s="199"/>
-      <c r="E33" s="199"/>
-      <c r="F33" s="199"/>
-      <c r="G33" s="199"/>
-      <c r="H33" s="199"/>
-      <c r="I33" s="199"/>
+      <c r="B33" s="195"/>
+      <c r="C33" s="195"/>
+      <c r="D33" s="202"/>
+      <c r="E33" s="202"/>
+      <c r="F33" s="202"/>
+      <c r="G33" s="202"/>
+      <c r="H33" s="202"/>
+      <c r="I33" s="202"/>
     </row>
   </sheetData>
   <mergeCells count="16">
+    <mergeCell ref="A1:I1"/>
+    <mergeCell ref="A2:I2"/>
+    <mergeCell ref="A3:I3"/>
+    <mergeCell ref="A4:I4"/>
+    <mergeCell ref="A5:B5"/>
+    <mergeCell ref="C5:G5"/>
+    <mergeCell ref="H5:I5"/>
     <mergeCell ref="A33:C33"/>
     <mergeCell ref="A7:C8"/>
     <mergeCell ref="D28:I33"/>
@@ -3487,13 +3494,6 @@
     <mergeCell ref="B10:D10"/>
     <mergeCell ref="A27:I27"/>
     <mergeCell ref="A28:C28"/>
-    <mergeCell ref="A1:I1"/>
-    <mergeCell ref="A2:I2"/>
-    <mergeCell ref="A3:I3"/>
-    <mergeCell ref="A4:I4"/>
-    <mergeCell ref="A5:B5"/>
-    <mergeCell ref="C5:G5"/>
-    <mergeCell ref="H5:I5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>